<commit_message>
projeto02 - feat e check
</commit_message>
<xml_diff>
--- a/PROJETOS/db-pipeline/assets/work_metadado_flights.xlsx
+++ b/PROJETOS/db-pipeline/assets/work_metadado_flights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Github/learn-python/PROJETOS/db-pipeline/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcamargg\Impacta\MBA_Impacta\PROJETOS\db-pipeline\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="11_AD4D361C20488DEA4E38A093BC5F47C25BDEDD84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3443CEFE-5955-4300-B4F4-9815EC8EF2BF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200A318C-27C8-4E2F-B65F-A219D80B424B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21697" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>tabela</t>
   </si>
@@ -121,6 +121,27 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>ano</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>mes</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -182,10 +203,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,23 +468,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C11" sqref="C11:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +513,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -525,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -554,7 +571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -583,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -612,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -641,7 +658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -670,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -699,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -728,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -757,18 +774,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G12" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>